<commit_message>
Main Thread Bug Whacked
</commit_message>
<xml_diff>
--- a/CAD/Robot v2/Robot BOM.xlsx
+++ b/CAD/Robot v2/Robot BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spyal\Documents\Arduino\ArduinoManufacturingRobots\CAD\Robot v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A8373-3A36-4228-A1CA-7E40C8C5742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45184416-7CEB-4F94-A782-11F61F6FE1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{E5D2AE15-C437-415D-9C0E-DFFC35D54DB3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Item</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Micro USB Jumper</t>
   </si>
   <si>
-    <t>https://www.parts-express.com/Panel-Mount-Micro-USB-Extension-Cable-Male-to-Female-130-031?quantity=1&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=18395892906&amp;utm_content=145242146127&amp;gadid=623430178298&amp;gclid=CjwKCAjwp6CkBhB_EiwAlQVyxbkmLhJTS6Z28GBJMspIRl-hFYwGrDVzzJEnQr-0v7eul_wmmSPeiBoCTYsQAvD_BwE</t>
-  </si>
-  <si>
     <t>LEDs</t>
   </si>
   <si>
@@ -195,6 +192,57 @@
   </si>
   <si>
     <t>Pack of 300, need ~40</t>
+  </si>
+  <si>
+    <t>Micro USB Cables</t>
+  </si>
+  <si>
+    <t>Colored 22 Gauge Wire</t>
+  </si>
+  <si>
+    <t>Heat Shrink</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CUI-Devices/CBL-UA-MUB-1?qs=l7cgNqFNU1hMub6kKPqayQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/3175/6198258</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/3m/FP-301-1-8-BL-500/116949</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/3258/6238006</t>
+  </si>
+  <si>
+    <t>Filament - Orange</t>
+  </si>
+  <si>
+    <t>Filament - Black</t>
+  </si>
+  <si>
+    <t>https://store.bambulab.com/products/pla-matte-filament?variant=40217021218931</t>
+  </si>
+  <si>
+    <t>https://store.bambulab.com/products/pla-basic-filament?variant=40820833648755</t>
+  </si>
+  <si>
+    <t>Solder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/american-beauty-tools/CS-PBF1/11685284</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/DFRobot/DFR0564?qs=%252BEew9%252B0nqrB%252BjqAikqlWKQ%3D%3D</t>
+  </si>
+  <si>
+    <t>7.4V Battery Charger</t>
+  </si>
+  <si>
+    <t>Qwicc Cable</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Adafruit/4210?qs=PzGy0jfpSMuCfezrcTX9rQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -618,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D0982-1D6A-4E08-978D-AFCA8FD7C91E}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -661,11 +709,11 @@
         <v>65.900000000000006</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:D18" si="0">C2*B2</f>
-        <v>65.900000000000006</v>
+        <f t="shared" ref="D2:D26" si="0">C2*B2</f>
+        <v>395.40000000000003</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -682,11 +730,11 @@
         <v>28.95</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>28.95</v>
+        <v>173.7</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -700,11 +748,11 @@
         <v>5.45</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>10.9</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -721,11 +769,11 @@
         <v>9.68</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>9.68</v>
+        <v>29.04</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -742,11 +790,11 @@
         <v>12.29</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>24.58</v>
+        <v>147.47999999999999</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -763,11 +811,11 @@
         <v>16.88</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>16.88</v>
+        <v>101.28</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -781,11 +829,11 @@
         <v>8.7899999999999991</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>8.7899999999999991</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -823,11 +871,11 @@
         <v>16.989999999999998</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>16.989999999999998</v>
+        <v>101.94</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
@@ -890,7 +938,7 @@
         <v>18.89</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>36</v>
@@ -925,11 +973,11 @@
         <v>11.99</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
-        <v>11.99</v>
+        <v>23.98</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -946,11 +994,11 @@
         <v>5.95</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="0"/>
-        <v>5.95</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="F16" t="s">
         <v>30</v>
@@ -958,23 +1006,23 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="5">
         <v>11.9</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="0"/>
-        <v>11.9</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -982,77 +1030,188 @@
         <v>46</v>
       </c>
       <c r="B18" s="5">
-        <v>4.49</v>
+        <v>4.95</v>
       </c>
       <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>24.75</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3.24</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>38.880000000000003</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="5">
+        <v>26.96</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>4.49</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>26.96</v>
+      </c>
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="5">
+        <v>15.74</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>15.74</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>49.98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="5">
+        <v>27.99</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>111.96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="5">
+        <v>7.06</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>7.06</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3">
-        <f>SUM(C2:C18)</f>
-        <v>19</v>
-      </c>
-      <c r="D20" s="6">
-        <f>SUM(D2:D18)</f>
-        <v>287.45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D24" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <f>SUM(C2:C19)</f>
+        <v>83</v>
+      </c>
+      <c r="D28" s="6">
+        <f>SUM(D2:D26)</f>
+        <v>1472.9800000000002</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1" display="https://www.amazon.com/Keadic-Embedment-Assortment-Fastening-Injection/dp/B08ZXSJN3H/ref=d_pd_di_sccai_cn_sccl_2_7/137-2949637-3098164?pd_rd_w=Ostb2&amp;content-id=amzn1.sym.e13de93e-5518-4644-8e6b-4ee5f2e0b062&amp;pf_rd_p=e13de93e-5518-4644-8e6b-4ee5f2e0b062&amp;pf_rd_r=MKAGC8DDN5KEJA2XD8V3&amp;pd_rd_wg=e4135&amp;pd_rd_r=859d181c-9947-456b-9948-f1ba3edb3bc2&amp;pd_rd_i=B08ZXSJN3H&amp;th=1" xr:uid="{7EAEE578-4302-40FC-9AC0-78B3A42341A0}"/>
-    <hyperlink ref="F18" r:id="rId2" display="https://www.parts-express.com/Panel-Mount-Micro-USB-Extension-Cable-Male-to-Female-130-031?quantity=1&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=18395892906&amp;utm_content=145242146127&amp;gadid=623430178298&amp;gclid=CjwKCAjwp6CkBhB_EiwAlQVyxbkmLhJTS6Z28GBJMspIRl-hFYwGrDVzzJEnQr-0v7eul_wmmSPeiBoCTYsQAvD_BwE" xr:uid="{B6C774F2-11EE-4341-913A-4F2731F642F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cd125eac-8659-41b2-94d0-26aa0a76da66" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008BEA995F60568D4FAB55D004B2A12D07" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e707669e86add063872c2c071ca7570a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd125eac-8659-41b2-94d0-26aa0a76da66" xmlns:ns4="e3782b96-feba-401b-bf66-07f33660656b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e671bce9bf202ca68324036394937c8" ns3:_="" ns4:_="">
     <xsd:import namespace="cd125eac-8659-41b2-94d0-26aa0a76da66"/>
@@ -1261,32 +1420,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7A0EB-61FF-4F93-84D4-01682163090D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e3782b96-feba-401b-bf66-07f33660656b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cd125eac-8659-41b2-94d0-26aa0a76da66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C056CD6-2967-4BA2-8261-A6EAE403C7EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cd125eac-8659-41b2-94d0-26aa0a76da66" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC201CA3-B6B9-4369-B443-EEDEF2B21021}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1303,4 +1454,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C056CD6-2967-4BA2-8261-A6EAE403C7EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7A0EB-61FF-4F93-84D4-01682163090D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3782b96-feba-401b-bf66-07f33660656b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cd125eac-8659-41b2-94d0-26aa0a76da66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>